<commit_message>
geological and structural model working
</commit_message>
<xml_diff>
--- a/data/data_geology/data_geology.xlsx
+++ b/data/data_geology/data_geology.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00105010\Projects\Gingin\data\data_geology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEF6D48-B4EB-459C-A858-147482CC91BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB5453C-ED69-4108-8FFB-A88F3C75B825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9A15C45E-C120-441D-BD00-A8D48E3A8925}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{9A15C45E-C120-441D-BD00-A8D48E3A8925}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="strat" sheetId="1" r:id="rId1"/>
     <sheet name="geo_bores" sheetId="2" r:id="rId2"/>
     <sheet name="pumping_bores" sheetId="3" r:id="rId3"/>
+    <sheet name="obs_bores" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="50">
   <si>
     <t>sequence</t>
   </si>
@@ -115,9 +116,6 @@
     <t>AM2</t>
   </si>
   <si>
-    <t>Editted</t>
-  </si>
-  <si>
     <t>Molecap Greensand</t>
   </si>
   <si>
@@ -146,13 +144,58 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>Jy</t>
+  </si>
+  <si>
+    <t>Yarragadee undifferentiated</t>
+  </si>
+  <si>
+    <t>Lancelin</t>
+  </si>
+  <si>
+    <t>Warnbro</t>
+  </si>
+  <si>
+    <t>Yarragadee</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Surface</t>
+  </si>
+  <si>
+    <t>OB1</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>AM1_upper</t>
+  </si>
+  <si>
+    <t>AM1_lower</t>
+  </si>
+  <si>
+    <t>AM2_upper</t>
+  </si>
+  <si>
+    <t>AM2_lower</t>
+  </si>
+  <si>
+    <t>made up</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +207,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -204,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -216,6 +266,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -552,16 +609,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25A2F9FB-DF61-4EEA-A974-F5C6A84730AC}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -589,13 +646,25 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="C2" s="6">
+        <v>255</v>
+      </c>
+      <c r="D2" s="6">
+        <v>255</v>
+      </c>
+      <c r="E2" s="6">
+        <v>255</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -604,87 +673,250 @@
         <v>-1</v>
       </c>
       <c r="H2" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="I2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
       </c>
+      <c r="C3" s="7">
+        <v>236</v>
+      </c>
+      <c r="D3" s="7">
+        <v>245</v>
+      </c>
+      <c r="E3" s="7">
+        <v>208</v>
+      </c>
+      <c r="F3">
+        <f>F2-H3</f>
+        <v>-100</v>
+      </c>
       <c r="G3">
         <v>0</v>
       </c>
+      <c r="H3">
+        <v>100</v>
+      </c>
       <c r="I3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
+      <c r="C4" s="7">
+        <v>171</v>
+      </c>
+      <c r="D4" s="7">
+        <v>198</v>
+      </c>
+      <c r="E4" s="7">
+        <v>184</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F10" si="0">F3-H4</f>
+        <v>-220</v>
+      </c>
       <c r="G4">
         <v>1</v>
       </c>
+      <c r="H4">
+        <v>120</v>
+      </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
+      <c r="C5" s="7">
+        <v>255</v>
+      </c>
+      <c r="D5" s="7">
+        <v>203</v>
+      </c>
+      <c r="E5" s="7">
+        <v>148</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>-310</v>
+      </c>
       <c r="G5">
         <v>2</v>
       </c>
+      <c r="H5">
+        <v>90</v>
+      </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
+      <c r="C6" s="7">
+        <v>89</v>
+      </c>
+      <c r="D6" s="7">
+        <v>139</v>
+      </c>
+      <c r="E6" s="7">
+        <v>93</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>-710</v>
+      </c>
       <c r="G6">
         <v>3</v>
       </c>
+      <c r="H6">
+        <v>400</v>
+      </c>
       <c r="I6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
       <c r="B7" t="s">
         <v>21</v>
       </c>
+      <c r="C7" s="7">
+        <v>148</v>
+      </c>
+      <c r="D7" s="7">
+        <v>139</v>
+      </c>
+      <c r="E7" s="7">
+        <v>83</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>-735</v>
+      </c>
       <c r="G7">
         <v>4</v>
       </c>
+      <c r="H7">
+        <v>25</v>
+      </c>
       <c r="I7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
       <c r="B8" t="s">
         <v>22</v>
       </c>
+      <c r="C8" s="7">
+        <v>79</v>
+      </c>
+      <c r="D8" s="7">
+        <v>98</v>
+      </c>
+      <c r="E8" s="7">
+        <v>51</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>-760</v>
+      </c>
       <c r="G8">
         <v>5</v>
       </c>
+      <c r="H8">
+        <v>25</v>
+      </c>
       <c r="I8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
+      <c r="C9" s="6">
+        <v>172</v>
+      </c>
+      <c r="D9" s="6">
+        <v>186</v>
+      </c>
+      <c r="E9" s="6">
+        <v>242</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>-1060</v>
+      </c>
       <c r="G9">
         <v>6</v>
       </c>
+      <c r="H9">
+        <v>300</v>
+      </c>
       <c r="I9" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="6">
+        <v>198</v>
+      </c>
+      <c r="D10" s="6">
+        <v>217</v>
+      </c>
+      <c r="E10" s="6">
+        <v>240</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>-1160</v>
+      </c>
+      <c r="G10">
+        <v>7</v>
+      </c>
+      <c r="H10">
+        <v>100</v>
+      </c>
+      <c r="I10" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -694,20 +926,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21C7B6E6-5797-4263-9D4F-99BD49F02BBF}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -747,8 +980,11 @@
       <c r="M1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -776,14 +1012,14 @@
       <c r="J2">
         <v>517</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="5">
         <v>517</v>
       </c>
       <c r="M2">
         <v>794</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -794,7 +1030,7 @@
         <v>6531829</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -808,17 +1044,23 @@
       <c r="H3">
         <v>218</v>
       </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
       <c r="J3">
         <v>517</v>
       </c>
       <c r="K3">
-        <v>517</v>
+        <v>535</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
       </c>
       <c r="M3">
         <v>794</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -852,8 +1094,11 @@
       <c r="L4">
         <v>829</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -864,7 +1109,7 @@
         <v>6529664</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
@@ -889,6 +1134,182 @@
       </c>
       <c r="L5">
         <v>829</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6">
+        <v>357097</v>
+      </c>
+      <c r="C6">
+        <v>6532212</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>99</v>
+      </c>
+      <c r="H6">
+        <v>218</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>517</v>
+      </c>
+      <c r="K6">
+        <v>535</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7">
+        <v>356786</v>
+      </c>
+      <c r="C7">
+        <v>6531447</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>99</v>
+      </c>
+      <c r="H7">
+        <v>218</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>517</v>
+      </c>
+      <c r="K7">
+        <v>535</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8">
+        <v>365763</v>
+      </c>
+      <c r="C8">
+        <v>6530013</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>123</v>
+      </c>
+      <c r="I8">
+        <v>210</v>
+      </c>
+      <c r="J8">
+        <v>775</v>
+      </c>
+      <c r="K8">
+        <v>803</v>
+      </c>
+      <c r="L8">
+        <v>829</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9">
+        <v>365568</v>
+      </c>
+      <c r="C9">
+        <v>6529285</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>123</v>
+      </c>
+      <c r="I9">
+        <v>210</v>
+      </c>
+      <c r="J9">
+        <v>775</v>
+      </c>
+      <c r="K9">
+        <v>803</v>
+      </c>
+      <c r="L9">
+        <v>829</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>881</v>
       </c>
     </row>
   </sheetData>
@@ -898,14 +1319,74 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B788AA5-15B1-4EC8-8CDF-DF3F9C64752D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2">
+        <v>362149</v>
+      </c>
+      <c r="C2">
+        <v>6530496</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{506D7985-1911-4924-B700-A70C8D504A68}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2">
+        <v>359649</v>
+      </c>
+      <c r="C2">
+        <v>6530996</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>